<commit_message>
feat: add updated raw and csv data
</commit_message>
<xml_diff>
--- a/raw data/Rivers and Lakes/Lakes - Rivers.xlsx
+++ b/raw data/Rivers and Lakes/Lakes - Rivers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artbo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artbo\Desktop\Project 2\raw data\Rivers and Lakes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53965A49-CB5C-4687-9C7B-D4DC331F1261}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32440B9-E92D-443F-B8F5-663285069918}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="45" windowWidth="16320" windowHeight="11940" xr2:uid="{19CB6955-7040-41BB-9526-146AE6753BB2}"/>
+    <workbookView xWindow="22500" yWindow="2160" windowWidth="16320" windowHeight="11940" xr2:uid="{19CB6955-7040-41BB-9526-146AE6753BB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -543,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -574,6 +574,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -891,7 +893,7 @@
   <dimension ref="B1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,7 +984,7 @@
       <c r="H4" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="24" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1005,7 +1007,7 @@
       <c r="H5" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="24" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1100,7 +1102,7 @@
       <c r="H9" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="24" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1255,7 +1257,7 @@
       <c r="F16" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="25" t="s">
         <v>70</v>
       </c>
       <c r="H16" s="11" t="s">

</xml_diff>

<commit_message>
docs: update river data sites w/in parameters (both metrics and start prior 2000)
</commit_message>
<xml_diff>
--- a/raw data/Rivers and Lakes/Lakes - Rivers.xlsx
+++ b/raw data/Rivers and Lakes/Lakes - Rivers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artbo\Desktop\Project 2\raw data\Rivers and Lakes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32440B9-E92D-443F-B8F5-663285069918}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DB3320-EB9B-436E-877B-57F433D0EA39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22500" yWindow="2160" windowWidth="16320" windowHeight="11940" xr2:uid="{19CB6955-7040-41BB-9526-146AE6753BB2}"/>
+    <workbookView xWindow="1035" yWindow="990" windowWidth="20265" windowHeight="15030" xr2:uid="{19CB6955-7040-41BB-9526-146AE6753BB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="156">
   <si>
     <t>Toledo Bend Reservoir</t>
   </si>
@@ -114,9 +114,6 @@
     <t>Canyon Lake</t>
   </si>
   <si>
-    <t>San Antonio</t>
-  </si>
-  <si>
     <t>Lavaca River</t>
   </si>
   <si>
@@ -156,15 +153,6 @@
     <t>Canadian River</t>
   </si>
   <si>
-    <t>El Paso</t>
-  </si>
-  <si>
-    <t>08475000</t>
-  </si>
-  <si>
-    <t>08364000</t>
-  </si>
-  <si>
     <t>Brownsville</t>
   </si>
   <si>
@@ -174,9 +162,6 @@
     <t>Gail</t>
   </si>
   <si>
-    <t>08162501</t>
-  </si>
-  <si>
     <t>Wadsworth</t>
   </si>
   <si>
@@ -186,18 +171,12 @@
     <t>Wayside</t>
   </si>
   <si>
-    <t>07331600</t>
-  </si>
-  <si>
     <t>Denison</t>
   </si>
   <si>
     <t>08088000</t>
   </si>
   <si>
-    <t>South Bend</t>
-  </si>
-  <si>
     <t>Amarillo</t>
   </si>
   <si>
@@ -216,12 +195,6 @@
     <t>Beaumont</t>
   </si>
   <si>
-    <t>08041780</t>
-  </si>
-  <si>
-    <t>Wills Point</t>
-  </si>
-  <si>
     <t>08017410</t>
   </si>
   <si>
@@ -252,9 +225,6 @@
     <t>Edna</t>
   </si>
   <si>
-    <t>08163500</t>
-  </si>
-  <si>
     <t>08164000</t>
   </si>
   <si>
@@ -345,54 +315,27 @@
     <t>08070000</t>
   </si>
   <si>
-    <t>Cleveland (E Fk)</t>
-  </si>
-  <si>
-    <t>08070200 </t>
-  </si>
-  <si>
     <t>New Caney (E Fk)</t>
   </si>
   <si>
-    <t>08030500 </t>
-  </si>
-  <si>
     <t>Ruliff</t>
   </si>
   <si>
-    <t>08211200 </t>
-  </si>
-  <si>
     <t>Bluntzer</t>
   </si>
   <si>
-    <t>08190000 </t>
-  </si>
-  <si>
     <t>Laguna</t>
   </si>
   <si>
-    <t>08067000 </t>
-  </si>
-  <si>
     <t>Liberty</t>
   </si>
   <si>
-    <t>08446500 </t>
-  </si>
-  <si>
     <t>Girvin</t>
   </si>
   <si>
-    <t>08176500 </t>
-  </si>
-  <si>
     <t>Victoria</t>
   </si>
   <si>
-    <t>08188500 </t>
-  </si>
-  <si>
     <t>Goliad</t>
   </si>
   <si>
@@ -406,13 +349,166 @@
   </si>
   <si>
     <t>Discharge, ft3/s</t>
+  </si>
+  <si>
+    <t>ElPaso</t>
+  </si>
+  <si>
+    <t>SouthBend</t>
+  </si>
+  <si>
+    <t>WillsPoint</t>
+  </si>
+  <si>
+    <t>Cleveland(EFk)</t>
+  </si>
+  <si>
+    <t>SanAntonio</t>
+  </si>
+  <si>
+    <t>Canadian Rv nr Amarillo, TX</t>
+  </si>
+  <si>
+    <t>Canadian Rv nr Canadian, TX</t>
+  </si>
+  <si>
+    <t>Pr Dog Twn Fk Red Rv nr Waysid</t>
+  </si>
+  <si>
+    <t>e, TX</t>
+  </si>
+  <si>
+    <t>Sabine Rv nr Wills Point, TX</t>
+  </si>
+  <si>
+    <t>Sabine Rv nr Ruliff, TX</t>
+  </si>
+  <si>
+    <t>Neches Rv nr Neches, TX</t>
+  </si>
+  <si>
+    <t>Trinity Rv bl Dallas, TX</t>
+  </si>
+  <si>
+    <t>Trinity Rv at Liberty, TX</t>
+  </si>
+  <si>
+    <t>E Fk San Jacinto Rv nr Clevela</t>
+  </si>
+  <si>
+    <t>nd, TX</t>
+  </si>
+  <si>
+    <t>E Fk San Jacinto Rv nr New Can</t>
+  </si>
+  <si>
+    <t>ey, TX</t>
+  </si>
+  <si>
+    <t>Brazos Rv nr South Bend, TX</t>
+  </si>
+  <si>
+    <t>Brazos Rv nr Rosharon, TX</t>
+  </si>
+  <si>
+    <t>Colorado Rv nr Gail, TX</t>
+  </si>
+  <si>
+    <t>Lavaca Rv nr Edna, TX</t>
+  </si>
+  <si>
+    <t>N Fk Guadalupe Rv nr Hunt, TX</t>
+  </si>
+  <si>
+    <t>Guadalupe Rv at Victoria, TX</t>
+  </si>
+  <si>
+    <t>San Antonio Rv at San Antonio,</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>San Antonio Rv at Goliad, TX</t>
+  </si>
+  <si>
+    <t>Nueces Rv at Laguna, TX</t>
+  </si>
+  <si>
+    <t>Nueces Rv at Bluntzer, TX</t>
+  </si>
+  <si>
+    <t>Pecos Rv nr Orla, TX</t>
+  </si>
+  <si>
+    <t>Pecos Rv nr Girvin, TX</t>
+  </si>
+  <si>
+    <t>08030500</t>
+  </si>
+  <si>
+    <t>08067000</t>
+  </si>
+  <si>
+    <t>08070200</t>
+  </si>
+  <si>
+    <t>08176500</t>
+  </si>
+  <si>
+    <t>08188500</t>
+  </si>
+  <si>
+    <t>08190000</t>
+  </si>
+  <si>
+    <t>08211200</t>
+  </si>
+  <si>
+    <t>08446500</t>
+  </si>
+  <si>
+    <t>08374550</t>
+  </si>
+  <si>
+    <t>Castolon</t>
+  </si>
+  <si>
+    <t>08375300</t>
+  </si>
+  <si>
+    <t>Big Bnd</t>
+  </si>
+  <si>
+    <t>Bay City</t>
+  </si>
+  <si>
+    <t>Burkburnett</t>
+  </si>
+  <si>
+    <t>08041000</t>
+  </si>
+  <si>
+    <t>Evadale</t>
+  </si>
+  <si>
+    <t>08162500</t>
+  </si>
+  <si>
+    <t>07308500</t>
+  </si>
+  <si>
+    <t>Rio Grande River * 2007</t>
+  </si>
+  <si>
+    <t>RIVER PARAMETERS - NEEDS TO HAVE BOTH GAGE HEIGHT AND DISCHARGE STARTING PRIOR TO 2000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -432,6 +528,21 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -543,7 +654,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -562,20 +673,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -890,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FBB076D-D139-4484-9013-421B8EB38CDC}">
-  <dimension ref="B1:K24"/>
+  <dimension ref="B1:Z38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,431 +1024,897 @@
     <col min="7" max="7" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="C1" s="23"/>
+    <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="29"/>
       <c r="F1" s="17" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="4" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E3" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="H3" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="I3" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="K3" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="L3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I4" s="24" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="K4" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" t="s">
+        <v>112</v>
+      </c>
+      <c r="M4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="I5" s="24" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="K5" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="L5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>53</v>
+        <v>106</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="K6" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="L6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="I7" s="21" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H7" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="K7" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="L7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>99</v>
+        <v>50</v>
+      </c>
+      <c r="K8" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="L8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>89</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>4</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="I9" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="K9" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="L9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="I10" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K10" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="L10" t="s">
+        <v>119</v>
+      </c>
+      <c r="M10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="I11" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="H11" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K11" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="L11" t="s">
+        <v>121</v>
+      </c>
+      <c r="M11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>114</v>
+        <v>54</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>143</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="K12" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="L12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="21" t="s">
-        <v>110</v>
+        <v>28</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>141</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="H13" s="21" t="s">
-        <v>108</v>
+        <v>96</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>142</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="K13" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="L13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H14" s="21" t="s">
-        <v>116</v>
+      <c r="H14" s="18" t="s">
+        <v>139</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="K14" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="L14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H15" s="21" t="s">
-        <v>118</v>
+        <v>109</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>140</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="K15" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="L15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="G16" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="H16" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="I16" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="K16" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="L16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B17" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="K17" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="L17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B18" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="22">
+        <f>COUNTIF($K$2:$K$23,F3)</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="H18" s="22">
+        <f>COUNTIF($K$2:$K$23,H3)</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="K18" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="L18" t="s">
+        <v>129</v>
+      </c>
+      <c r="M18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="22">
+        <f t="shared" ref="F19:H30" si="0">COUNTIF($K$2:$K$23,F4)</f>
+        <v>1</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H19" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="K19" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="L19" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B20" s="15" t="s">
         <v>24</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H20" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="K20" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="L20" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B21" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="H21" s="22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="K21" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="L21" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B22" s="15" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" s="22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I22" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="K22" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="L22" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B23" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H23" s="22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="K23" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="L23" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>80</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="E25" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="H25" s="22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="M25" s="2">
+        <v>8364000</v>
+      </c>
+      <c r="N25">
+        <v>8117995</v>
+      </c>
+      <c r="O25">
+        <v>7297910</v>
+      </c>
+      <c r="P25">
+        <v>8088000</v>
+      </c>
+      <c r="Q25">
+        <v>8057410</v>
+      </c>
+      <c r="R25">
+        <v>7227500</v>
+      </c>
+      <c r="S25">
+        <v>8032000</v>
+      </c>
+      <c r="T25">
+        <v>8017410</v>
+      </c>
+      <c r="U25">
+        <v>8070000</v>
+      </c>
+      <c r="V25">
+        <v>8412500</v>
+      </c>
+      <c r="W25">
+        <v>8190000</v>
+      </c>
+      <c r="X25">
+        <v>8165300</v>
+      </c>
+      <c r="Y25">
+        <v>8178000</v>
+      </c>
+      <c r="Z25">
+        <v>8163500</v>
+      </c>
+    </row>
+    <row r="26" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="E26" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" s="22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="H26" s="22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="E27" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H27" s="22">
+        <f>COUNTIF($K$2:$K$23,H12)</f>
+        <v>1</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="E28" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="H28" s="22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="E29" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F29" s="22">
+        <f>COUNTIF($K$2:$K$23,F14)</f>
+        <v>1</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H29" s="22">
+        <f>COUNTIF($K$2:$K$23,H14)</f>
+        <v>1</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="E30" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F30" s="22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H30" s="22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E31" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" s="22">
+        <f>COUNTIF($K$2:$K$23,F16)</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="H31" s="22">
+        <f>COUNTIF($K$2:$K$23,H16)</f>
+        <v>1</v>
+      </c>
+      <c r="I31" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
+    </row>
+    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E33" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="F33" s="22"/>
+    </row>
+    <row r="34" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F34" s="22"/>
+    </row>
+    <row r="35" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F35" s="22"/>
+    </row>
+    <row r="36" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F36" s="22"/>
+    </row>
+    <row r="37" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F37" s="22"/>
+    </row>
+    <row r="38" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F38" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>